<commit_message>
task 20 to task 27
</commit_message>
<xml_diff>
--- a/SourceCode/2024/Basics-April2024/hasini/task 20/input.xlsx
+++ b/SourceCode/2024/Basics-April2024/hasini/task 20/input.xlsx
@@ -14,6 +14,7 @@
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <x:sheet name="sheet2" sheetId="5" r:id="rId5"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="162913"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <x:si>
     <x:t>lowercase</x:t>
   </x:si>
@@ -50,6 +51,21 @@
   </x:si>
   <x:si>
     <x:t>FGH</x:t>
+  </x:si>
+  <x:si>
+    <x:t>lower case</x:t>
+  </x:si>
+  <x:si>
+    <x:t>upper case</x:t>
+  </x:si>
+  <x:si>
+    <x:t>status</x:t>
+  </x:si>
+  <x:si>
+    <x:t>text</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Success</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -429,4 +445,73 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:C4"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:3">
+      <x:c r="A1" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:3">
+      <x:c r="A2" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3">
+      <x:c r="A3" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:3">
+      <x:c r="A4" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:3">
+      <x:c r="A5" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>